<commit_message>
st: updated TAS1 forms
</commit_message>
<xml_diff>
--- a/LF/TAS/STP/st_lf_tas1_2_partcipants_202204.xlsx
+++ b/LF/TAS/STP/st_lf_tas1_2_partcipants_202204.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>type</t>
   </si>
@@ -24,10 +24,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>label::English</t>
-  </si>
-  <si>
-    <t>hint::English</t>
+    <t>label::Portugese</t>
+  </si>
+  <si>
+    <t>hint::Portugese</t>
   </si>
   <si>
     <t>label::French</t>
@@ -42,7 +42,7 @@
     <t>constraint</t>
   </si>
   <si>
-    <t>constraint_message::English</t>
+    <t>constraint_message::Portugese</t>
   </si>
   <si>
     <t>constraint_message::French</t>
@@ -72,10 +72,10 @@
     <t>p_recorderID</t>
   </si>
   <si>
-    <t>Enter Recorder ID</t>
-  </si>
-  <si>
-    <t>If you are the only recorder on your team, this may be called a "team ID". Recorder ID is the 2-digit code assigned to you or your team.</t>
+    <t>Introduzir o ID do gravador</t>
+  </si>
+  <si>
+    <t>Se for o único gravador da sua equipa, este pode ser chamado de "identificação da equipa". O ID do gravador é um código de 2 dígitos que lhe foi atribuído a si ou à sua equipa.</t>
   </si>
   <si>
     <t>Entrer l'identifiant de l'enregistreur</t>
@@ -87,7 +87,7 @@
     <t>regex(.,'^[0-9]{2}$')</t>
   </si>
   <si>
-    <t>The code must be a two-digit number between 9 and 100</t>
+    <t>O código deve ser um número de dois algarismos entre 9 e 100</t>
   </si>
   <si>
     <t>Le code doit être un nombre à deux chiffres entre 9 et 100</t>
@@ -102,37 +102,43 @@
     <t>p_eu_name</t>
   </si>
   <si>
-    <t>Select your evaluation unit (EU)</t>
+    <t>Seleccionar província</t>
+  </si>
+  <si>
+    <t>Sélectionner la province</t>
+  </si>
+  <si>
+    <t>p_district</t>
+  </si>
+  <si>
+    <t>Seleccionar a unidade de avaliação</t>
   </si>
   <si>
     <t>Sélectionner l'unité d'évaluation (UE)</t>
   </si>
   <si>
-    <t>p_commune</t>
-  </si>
-  <si>
-    <t>Select your commune</t>
-  </si>
-  <si>
-    <t>Sélectionner votre commune</t>
-  </si>
-  <si>
     <t>p_cluster_name</t>
   </si>
   <si>
-    <t>Select your school name</t>
-  </si>
-  <si>
-    <t>Sélectionner votre école</t>
+    <t>Introduza o nome do local</t>
+  </si>
+  <si>
+    <t>Entrer le nom de la localité</t>
   </si>
   <si>
     <t>p_cluster_id</t>
   </si>
   <si>
-    <t>Select your school id</t>
-  </si>
-  <si>
-    <t>Sélectionner le code de votre école</t>
+    <t>Introduza o código da localidade</t>
+  </si>
+  <si>
+    <t>O código de três dígitos associado a cada local</t>
+  </si>
+  <si>
+    <t>Entrer le code de la localité</t>
+  </si>
+  <si>
+    <t>Le code a trois chiffres associés à chaque localité</t>
   </si>
   <si>
     <t>select_one yes_no</t>
@@ -141,7 +147,7 @@
     <t>p_consent</t>
   </si>
   <si>
-    <t>Does respondent provide consent?</t>
+    <t>O inquirido dá o seu consentimento?</t>
   </si>
   <si>
     <t>Le répondant a-t-il donné son consentement?</t>
@@ -153,37 +159,37 @@
     <t>p_sex</t>
   </si>
   <si>
-    <t>Sex of respondent</t>
+    <t>Sexo do inquirido</t>
   </si>
   <si>
     <t>Sexe du participant</t>
   </si>
   <si>
-    <t>${p_consent} = 'Yes'</t>
+    <t>${p_consent} = 'Sim'</t>
   </si>
   <si>
     <t>p_age_yrs</t>
   </si>
   <si>
-    <t>Enter age in years</t>
+    <t>Introduzir a idade em anos</t>
   </si>
   <si>
     <t>Entrer l'âge du participant (en années)</t>
   </si>
   <si>
-    <t>. &gt;= 5 and . &lt;= 9</t>
-  </si>
-  <si>
-    <t>The age must be between 5 and 9 years</t>
-  </si>
-  <si>
-    <t>L'age doit être compris entre 5 et 9 ans</t>
+    <t>. &gt;= 5 and . &lt;= 21</t>
+  </si>
+  <si>
+    <t>A idade deve ser entre os 5 e 21 anos</t>
+  </si>
+  <si>
+    <t>L'age doit être compris entre 5 et 21 ans</t>
   </si>
   <si>
     <t>p_how_long_lived</t>
   </si>
   <si>
-    <t>How many years has the respondent lived in the area?</t>
+    <t>Quantos anos viveu o inquirido na zona?</t>
   </si>
   <si>
     <t>Depuis combien d'années le participant habite-t-il dans la communauté?</t>
@@ -192,7 +198,7 @@
     <t>. &lt;= ${p_age_yrs}</t>
   </si>
   <si>
-    <t>The value must not be greater than the age</t>
+    <t>O valor não deve ser maior do que a idade</t>
   </si>
   <si>
     <t>La valeur ne doit pas être supérieure à l'âge</t>
@@ -204,7 +210,7 @@
     <t>p_IDMethod</t>
   </si>
   <si>
-    <t>How will the individual's unique ID be generated?</t>
+    <t>Como será gerada a identificação única do indivíduo?</t>
   </si>
   <si>
     <t>Comment l'ID unique de l'individu sera-t-il généré?</t>
@@ -216,25 +222,25 @@
     <t>p_BarcodeID</t>
   </si>
   <si>
-    <t>Scan barcode now</t>
+    <t>Digitalize agora o código de barras</t>
   </si>
   <si>
     <t>Scanner le code-barres maintenant</t>
   </si>
   <si>
-    <t>${p_IDMethod} = 'Scanner' and ${p_consent} = 'Yes'</t>
+    <t>${p_IDMethod} = 'Scanner' and ${p_consent} = 'Sim'</t>
   </si>
   <si>
     <t>p_GenerateID</t>
   </si>
   <si>
-    <t>Please record the following unique ID code for the respondent on a separate list and on each diagnostic test(s) administered</t>
+    <t>Registar o seguinte código de identificação único para o respondente numa lista separada e em cada teste(s) de diagnóstico administrado(s)</t>
   </si>
   <si>
     <t>Veuiller enregistrer le code d'identification unique du participant qui apparait sur une liste séparée et sur chaque test de diagnostic administré</t>
   </si>
   <si>
-    <t>${p_IDMethod} = 'ID_generation' and ${p_consent} = 'Yes'</t>
+    <t>${p_IDMethod} = 'ID_generation' and ${p_consent} = 'Sim'</t>
   </si>
   <si>
     <t>concat(${p_cluster_id},'-',substr(random(),3,10))</t>
@@ -246,13 +252,13 @@
     <t>p_ending_survey_note</t>
   </si>
   <si>
-    <t>You just entered a value that will end the survey</t>
+    <t>Acaba de introduzir um valor que terminará o inquérito</t>
   </si>
   <si>
     <t>Vous vener de saisir une valeur qui mettra fin à l'enquête</t>
   </si>
   <si>
-    <t>${p_consent} = 'No'</t>
+    <t>${p_consent} = 'Nao'</t>
   </si>
   <si>
     <t>text</t>
@@ -261,7 +267,7 @@
     <t>p_notes</t>
   </si>
   <si>
-    <t>Additional Notes</t>
+    <t>Notas Adicionais</t>
   </si>
   <si>
     <t>Notes complémentaires</t>
@@ -270,13 +276,13 @@
     <t>start</t>
   </si>
   <si>
-    <t>c_start</t>
+    <t>p_start</t>
   </si>
   <si>
     <t>end</t>
   </si>
   <si>
-    <t>c_end</t>
+    <t>p_end</t>
   </si>
   <si>
     <t>list_name</t>
@@ -285,13 +291,13 @@
     <t>yes_no</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>Sim</t>
   </si>
   <si>
     <t>Oui</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Nao</t>
   </si>
   <si>
     <t>Non</t>
@@ -300,13 +306,13 @@
     <t>sex_list</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Masculino</t>
   </si>
   <si>
     <t>Masculin</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Feminino</t>
   </si>
   <si>
     <t>Féminin</t>
@@ -321,7 +327,7 @@
     <t>ID_generation</t>
   </si>
   <si>
-    <t>Automatic ID generation</t>
+    <t>Geração automática</t>
   </si>
   <si>
     <t>Génération automatique</t>
@@ -339,13 +345,13 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Fev 2022) 2. TAS1 FL - Formulaire Participants V2</t>
-  </si>
-  <si>
-    <t>sn_lf_tas1_2_partcipants_202202_2</t>
-  </si>
-  <si>
-    <t>French</t>
+    <t>(Abr 2022) 2. TAS1 FL - Formulário de participantes</t>
+  </si>
+  <si>
+    <t>st_lf_tas1_2_partcipants_202204</t>
+  </si>
+  <si>
+    <t>Portugese</t>
   </si>
 </sst>
 </file>
@@ -353,9 +359,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
@@ -416,8 +422,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,23 +506,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -463,94 +538,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -573,187 +579,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,36 +803,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -848,21 +828,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -877,11 +842,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -897,118 +903,118 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1017,22 +1023,22 @@
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1441,12 +1447,12 @@
   <sheetPr/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="$A3:$XFD6"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1468,7 +1474,7 @@
     <col min="16" max="16" width="36.6222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="18" spans="1:16">
+    <row r="1" s="3" customFormat="1" ht="36" spans="1:16">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1650,11 +1656,15 @@
       <c r="C6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="E6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="15"/>
+        <v>39</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="28"/>
@@ -1668,17 +1678,17 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:16">
       <c r="A7" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="13"/>
@@ -1696,17 +1706,17 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="1:16">
       <c r="A8" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="13"/>
@@ -1714,7 +1724,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="12"/>
       <c r="K8" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13" t="s">
@@ -1729,28 +1739,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13" t="s">
@@ -1765,28 +1775,28 @@
         <v>16</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="13" t="s">
@@ -1796,19 +1806,19 @@
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
     </row>
-    <row r="11" s="3" customFormat="1" spans="1:16">
+    <row r="11" s="3" customFormat="1" ht="28.5" spans="1:16">
       <c r="A11" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="12"/>
@@ -1816,7 +1826,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L11" s="12"/>
       <c r="M11" s="13" t="s">
@@ -1828,17 +1838,17 @@
     </row>
     <row r="12" s="3" customFormat="1" spans="1:16">
       <c r="A12" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="12"/>
@@ -1846,7 +1856,7 @@
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="13" t="s">
@@ -1861,14 +1871,14 @@
         <v>26</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="12"/>
@@ -1876,10 +1886,10 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M13" s="13" t="s">
         <v>25</v>
@@ -1892,17 +1902,17 @@
     </row>
     <row r="14" s="3" customFormat="1" ht="28.5" spans="1:16">
       <c r="A14" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="12"/>
@@ -1910,7 +1920,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="13"/>
@@ -1920,17 +1930,17 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:16">
       <c r="A15" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="12"/>
@@ -1946,10 +1956,10 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:16">
       <c r="A16" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -1968,10 +1978,10 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -2003,7 +2013,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="4"/>
@@ -2016,7 +2026,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -2031,86 +2041,86 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2127,8 +2137,8 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2140,30 +2150,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2">
         <v>20210419</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>